<commit_message>
modified tab names to correspond to class names
</commit_message>
<xml_diff>
--- a/docs/physParams/UnifiedParameters.xlsx
+++ b/docs/physParams/UnifiedParameters.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\radtrack\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\radtrack\docs\physParams\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24795" windowHeight="11910" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24795" windowHeight="11910" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="UndC" sheetId="1" r:id="rId1"/>
-    <sheet name="BeamP" sheetId="2" r:id="rId2"/>
-    <sheet name="Precision" sheetId="3" r:id="rId3"/>
-    <sheet name="Wavefront" sheetId="4" r:id="rId4"/>
-    <sheet name="Radiation" sheetId="5" r:id="rId5"/>
-    <sheet name="EBeamline" sheetId="6" r:id="rId6"/>
-    <sheet name="LBeamline" sheetId="7" r:id="rId7"/>
+    <sheet name="undulator" sheetId="1" r:id="rId1"/>
+    <sheet name="particleBeam" sheetId="2" r:id="rId2"/>
+    <sheet name="precisionSRW" sheetId="3" r:id="rId3"/>
+    <sheet name="wavefrontSRW" sheetId="4" r:id="rId4"/>
+    <sheet name="bunchTransportTab" sheetId="6" r:id="rId5"/>
+    <sheet name="laserTransportTab" sheetId="7" r:id="rId6"/>
+    <sheet name="laserTab" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1939,7 +1939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -3337,7 +3337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -3349,7 +3349,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -3361,9 +3363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>